<commit_message>
append result of 刘思柒
</commit_message>
<xml_diff>
--- a/test-result/vector/test-result-on-linux.xlsx
+++ b/test-result/vector/test-result-on-linux.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="test-result-on-linux" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>515021910153_盛佩瑶</t>
   </si>
@@ -241,6 +241,17 @@
   </si>
   <si>
     <t>total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>515030910406_刘思柒</t>
+  </si>
+  <si>
+    <t>Failed(WA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Failed(RE)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -578,7 +589,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -698,15 +709,15 @@
         <v>2147483647</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K15" si="0">$J$17/J3</f>
+        <f t="shared" ref="K3:K16" si="0">$J$17/J3</f>
         <v>1.4016404754489848E-9</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L15" si="1">20*K3</f>
+        <f t="shared" ref="L3:L16" si="1">20*K3</f>
         <v>2.8032809508979695E-8</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M15" si="2">D3+G3+L3</f>
+        <f t="shared" ref="M3:M16" si="2">D3+G3+L3</f>
         <v>2.8032809508979695E-8</v>
       </c>
     </row>
@@ -1167,15 +1178,42 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="2">
+        <v>20</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="I16" s="2"/>
+      <c r="J16" s="1">
+        <v>2147483647</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4016404754489848E-9</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8032809508979695E-8</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>20.000000028032808</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J17" s="1">

</xml_diff>